<commit_message>
Add Book4.xlsx and update processed data files
Added Book4.xlsx and updated dif_medias_staggered.xlsx in processed data. Removed temporary Excel files and updated several .DS_Store files.
</commit_message>
<xml_diff>
--- a/data/controles_results/processed/dif_medias_staggered.xlsx
+++ b/data/controles_results/processed/dif_medias_staggered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiaaristizabal/Desktop/1 economia/7/econometría avanzada/proyecto_econometria_avanzada/data/controles_results/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92697A00-3F13-A84C-860C-33A4DADEB9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971C8E28-DFE3-CD46-82DC-861ABA19DF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12660" yWindow="500" windowWidth="16120" windowHeight="15620" xr2:uid="{663163B4-16DE-5547-829E-8B80DC7B8A56}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="71">
   <si>
     <t/>
   </si>
@@ -643,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8E877C-4FB4-814D-BE68-93388D02FBDD}">
   <dimension ref="B2:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -663,9 +663,7 @@
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
         <v>13</v>
       </c>

</xml_diff>